<commit_message>
started the 1-in test
</commit_message>
<xml_diff>
--- a/data 10242016.xlsx
+++ b/data 10242016.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="23955" windowHeight="9525"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="20730" windowHeight="9525" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="10-24 testing" sheetId="1" r:id="rId1"/>
+    <sheet name="10-26 testing" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="7">
   <si>
     <t>Position</t>
   </si>
@@ -52,7 +52,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,6 +77,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -90,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -99,6 +105,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="I4" workbookViewId="0">
+      <selection sqref="A1:AA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -981,11 +988,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="M5:M22"/>
-    <mergeCell ref="O5:O22"/>
-    <mergeCell ref="T5:T22"/>
-    <mergeCell ref="V5:V22"/>
-    <mergeCell ref="AA5:AA22"/>
     <mergeCell ref="H1:M3"/>
     <mergeCell ref="O1:T3"/>
     <mergeCell ref="A1:F3"/>
@@ -993,6 +995,11 @@
     <mergeCell ref="A5:A22"/>
     <mergeCell ref="F5:F22"/>
     <mergeCell ref="H5:H22"/>
+    <mergeCell ref="M5:M22"/>
+    <mergeCell ref="O5:O22"/>
+    <mergeCell ref="T5:T22"/>
+    <mergeCell ref="V5:V22"/>
+    <mergeCell ref="AA5:AA22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1000,12 +1007,1354 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AA28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="0.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="0.5703125" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="0.7109375" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>85.4</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>87.6</v>
+      </c>
+      <c r="L5">
+        <v>25</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>91.1</v>
+      </c>
+      <c r="S5">
+        <v>25</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" s="4"/>
+      <c r="V5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>87.2</v>
+      </c>
+      <c r="Z5">
+        <v>25</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="2"/>
+      <c r="B6">
+        <f>B5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>82.4</v>
+      </c>
+      <c r="E6">
+        <f>E5+1</f>
+        <v>26</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="2"/>
+      <c r="I6">
+        <f>I5+1</f>
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>84.8</v>
+      </c>
+      <c r="L6">
+        <f>L5+1</f>
+        <v>26</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="2"/>
+      <c r="P6">
+        <f>P5+1</f>
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>88.6</v>
+      </c>
+      <c r="S6">
+        <f>S5+1</f>
+        <v>26</v>
+      </c>
+      <c r="T6" s="2"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="2"/>
+      <c r="W6">
+        <f>W5+1</f>
+        <v>2</v>
+      </c>
+      <c r="Y6">
+        <v>85.2</v>
+      </c>
+      <c r="Z6">
+        <f>Z5+1</f>
+        <v>26</v>
+      </c>
+      <c r="AA6" s="2"/>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" s="2"/>
+      <c r="B7">
+        <f t="shared" ref="B7:B28" si="0">B6+1</f>
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E28" si="1">E6+1</f>
+        <v>27</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="2"/>
+      <c r="I7">
+        <f t="shared" ref="I7:I28" si="2">I6+1</f>
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>81.5</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ref="L7:L28" si="3">L6+1</f>
+        <v>27</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="2"/>
+      <c r="P7">
+        <f t="shared" ref="P7:P28" si="4">P6+1</f>
+        <v>3</v>
+      </c>
+      <c r="R7">
+        <v>85.5</v>
+      </c>
+      <c r="S7">
+        <f t="shared" ref="S7:S28" si="5">S6+1</f>
+        <v>27</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="2"/>
+      <c r="W7">
+        <f t="shared" ref="W7:W28" si="6">W6+1</f>
+        <v>3</v>
+      </c>
+      <c r="Y7">
+        <v>82.2</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" ref="Z7:Z28" si="7">Z6+1</f>
+        <v>27</v>
+      </c>
+      <c r="AA7" s="2"/>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" s="2"/>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="2"/>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="2"/>
+      <c r="P8">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="2"/>
+      <c r="W8">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="7"/>
+        <v>28</v>
+      </c>
+      <c r="AA8" s="2"/>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" s="2"/>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="2"/>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="2"/>
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="T9" s="2"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="2"/>
+      <c r="W9">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="7"/>
+        <v>29</v>
+      </c>
+      <c r="AA9" s="2"/>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="A10" s="2"/>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="2"/>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="2"/>
+      <c r="P10">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="T10" s="2"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="2"/>
+      <c r="W10">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="AA10" s="2"/>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11" s="2"/>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="2"/>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="2"/>
+      <c r="P11">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="5"/>
+        <v>31</v>
+      </c>
+      <c r="T11" s="2"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="2"/>
+      <c r="W11">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="7"/>
+        <v>31</v>
+      </c>
+      <c r="AA11" s="2"/>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12" s="2"/>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="2"/>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="2"/>
+      <c r="P12">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="T12" s="2"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="2"/>
+      <c r="W12">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="7"/>
+        <v>32</v>
+      </c>
+      <c r="AA12" s="2"/>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13" s="2"/>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="2"/>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="2"/>
+      <c r="P13">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
+      <c r="T13" s="2"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="2"/>
+      <c r="W13">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="7"/>
+        <v>33</v>
+      </c>
+      <c r="AA13" s="2"/>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14" s="2"/>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="2"/>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="2"/>
+      <c r="P14">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="5"/>
+        <v>34</v>
+      </c>
+      <c r="T14" s="2"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="2"/>
+      <c r="W14">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="7"/>
+        <v>34</v>
+      </c>
+      <c r="AA14" s="2"/>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="A15" s="2"/>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="2"/>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="2"/>
+      <c r="P15">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="T15" s="2"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="2"/>
+      <c r="W15">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="7"/>
+        <v>35</v>
+      </c>
+      <c r="AA15" s="2"/>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="A16" s="2"/>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="2"/>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="2"/>
+      <c r="P16">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="T16" s="2"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="2"/>
+      <c r="W16">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="7"/>
+        <v>36</v>
+      </c>
+      <c r="AA16" s="2"/>
+    </row>
+    <row r="17" spans="1:27">
+      <c r="A17" s="2"/>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="2"/>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="2"/>
+      <c r="P17">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="5"/>
+        <v>37</v>
+      </c>
+      <c r="T17" s="2"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="2"/>
+      <c r="W17">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="7"/>
+        <v>37</v>
+      </c>
+      <c r="AA17" s="2"/>
+    </row>
+    <row r="18" spans="1:27">
+      <c r="A18" s="2"/>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="2"/>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="2"/>
+      <c r="P18">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="5"/>
+        <v>38</v>
+      </c>
+      <c r="T18" s="2"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="2"/>
+      <c r="W18">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="7"/>
+        <v>38</v>
+      </c>
+      <c r="AA18" s="2"/>
+    </row>
+    <row r="19" spans="1:27">
+      <c r="A19" s="2"/>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="2"/>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="2"/>
+      <c r="P19">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="5"/>
+        <v>39</v>
+      </c>
+      <c r="T19" s="2"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="2"/>
+      <c r="W19">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="7"/>
+        <v>39</v>
+      </c>
+      <c r="AA19" s="2"/>
+    </row>
+    <row r="20" spans="1:27">
+      <c r="A20" s="2"/>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="2"/>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="2"/>
+      <c r="P20">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="T20" s="2"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="2"/>
+      <c r="W20">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+      <c r="AA20" s="2"/>
+    </row>
+    <row r="21" spans="1:27">
+      <c r="A21" s="2"/>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="2"/>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="2"/>
+      <c r="P21">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="5"/>
+        <v>41</v>
+      </c>
+      <c r="T21" s="2"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="2"/>
+      <c r="W21">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" si="7"/>
+        <v>41</v>
+      </c>
+      <c r="AA21" s="2"/>
+    </row>
+    <row r="22" spans="1:27">
+      <c r="A22" s="2"/>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="2"/>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="2"/>
+      <c r="P22">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+      <c r="T22" s="2"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="2"/>
+      <c r="W22">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="Z22">
+        <f t="shared" si="7"/>
+        <v>42</v>
+      </c>
+      <c r="AA22" s="2"/>
+    </row>
+    <row r="23" spans="1:27">
+      <c r="A23" s="2"/>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="2"/>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="2"/>
+      <c r="P23">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="5"/>
+        <v>43</v>
+      </c>
+      <c r="T23" s="2"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="2"/>
+      <c r="W23">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" si="7"/>
+        <v>43</v>
+      </c>
+      <c r="AA23" s="2"/>
+    </row>
+    <row r="24" spans="1:27">
+      <c r="A24" s="2"/>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="2"/>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="2"/>
+      <c r="P24">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="5"/>
+        <v>44</v>
+      </c>
+      <c r="T24" s="2"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="2"/>
+      <c r="W24">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="7"/>
+        <v>44</v>
+      </c>
+      <c r="AA24" s="2"/>
+    </row>
+    <row r="25" spans="1:27">
+      <c r="A25" s="2"/>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="2"/>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="2"/>
+      <c r="P25">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="5"/>
+        <v>45</v>
+      </c>
+      <c r="T25" s="2"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="2"/>
+      <c r="W25">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="AA25" s="2"/>
+    </row>
+    <row r="26" spans="1:27">
+      <c r="A26" s="2"/>
+      <c r="B26">
+        <f>B25+1</f>
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>76.7</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="2"/>
+      <c r="I26">
+        <f>I25+1</f>
+        <v>22</v>
+      </c>
+      <c r="J26">
+        <v>63.5</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="2"/>
+      <c r="P26">
+        <f>P25+1</f>
+        <v>22</v>
+      </c>
+      <c r="Q26">
+        <v>62.1</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="5"/>
+        <v>46</v>
+      </c>
+      <c r="T26" s="2"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="2"/>
+      <c r="W26">
+        <f>W25+1</f>
+        <v>22</v>
+      </c>
+      <c r="X26">
+        <v>56.2</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" si="7"/>
+        <v>46</v>
+      </c>
+      <c r="AA26" s="2"/>
+    </row>
+    <row r="27" spans="1:27">
+      <c r="A27" s="2"/>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C27">
+        <v>79.900000000000006</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="2"/>
+      <c r="I27">
+        <f t="shared" ref="I27:I28" si="8">I26+1</f>
+        <v>23</v>
+      </c>
+      <c r="J27">
+        <v>66.7</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="2"/>
+      <c r="P27">
+        <f t="shared" ref="P27:P28" si="9">P26+1</f>
+        <v>23</v>
+      </c>
+      <c r="Q27">
+        <v>62.7</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="5"/>
+        <v>47</v>
+      </c>
+      <c r="T27" s="2"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="2"/>
+      <c r="W27">
+        <f t="shared" ref="W27:W28" si="10">W26+1</f>
+        <v>23</v>
+      </c>
+      <c r="X27">
+        <v>57.5</v>
+      </c>
+      <c r="Z27">
+        <f t="shared" si="7"/>
+        <v>47</v>
+      </c>
+      <c r="AA27" s="2"/>
+    </row>
+    <row r="28" spans="1:27">
+      <c r="A28" s="2"/>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C28">
+        <v>82</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="2"/>
+      <c r="I28">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+      <c r="J28">
+        <v>69</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="2"/>
+      <c r="P28">
+        <f t="shared" si="9"/>
+        <v>24</v>
+      </c>
+      <c r="Q28">
+        <v>64</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="T28" s="2"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="2"/>
+      <c r="W28">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="X28">
+        <v>58</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" si="7"/>
+        <v>48</v>
+      </c>
+      <c r="AA28" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A5:A28"/>
+    <mergeCell ref="F5:F28"/>
+    <mergeCell ref="H5:H28"/>
+    <mergeCell ref="M5:M28"/>
+    <mergeCell ref="O5:O28"/>
+    <mergeCell ref="T5:T28"/>
+    <mergeCell ref="V5:V28"/>
+    <mergeCell ref="AA5:AA28"/>
+    <mergeCell ref="A1:F3"/>
+    <mergeCell ref="H1:M3"/>
+    <mergeCell ref="O1:T3"/>
+    <mergeCell ref="V1:AA3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added more 1-in data
</commit_message>
<xml_diff>
--- a/data 10242016.xlsx
+++ b/data 10242016.xlsx
@@ -52,7 +52,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,6 +83,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -96,16 +102,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,7 +558,7 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B5">
@@ -566,10 +573,10 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I5">
@@ -584,10 +591,10 @@
       <c r="L5">
         <v>1</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="O5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="P5">
@@ -602,10 +609,10 @@
       <c r="S5">
         <v>1</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="T5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="V5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="W5">
@@ -620,12 +627,12 @@
       <c r="Z5">
         <v>1</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="AA5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="2"/>
+      <c r="A6" s="4"/>
       <c r="B6">
         <v>7</v>
       </c>
@@ -638,8 +645,8 @@
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="F6" s="4"/>
+      <c r="H6" s="4"/>
       <c r="I6">
         <v>7</v>
       </c>
@@ -652,8 +659,8 @@
       <c r="L6">
         <v>2</v>
       </c>
-      <c r="M6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="M6" s="4"/>
+      <c r="O6" s="4"/>
       <c r="P6">
         <v>7</v>
       </c>
@@ -666,8 +673,8 @@
       <c r="S6">
         <v>2</v>
       </c>
-      <c r="T6" s="2"/>
-      <c r="V6" s="2"/>
+      <c r="T6" s="4"/>
+      <c r="V6" s="4"/>
       <c r="W6">
         <v>7</v>
       </c>
@@ -680,10 +687,10 @@
       <c r="Z6">
         <v>2</v>
       </c>
-      <c r="AA6" s="2"/>
+      <c r="AA6" s="4"/>
     </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="2"/>
+      <c r="A7" s="4"/>
       <c r="B7">
         <v>8</v>
       </c>
@@ -696,8 +703,8 @@
       <c r="E7">
         <v>3</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="F7" s="4"/>
+      <c r="H7" s="4"/>
       <c r="I7">
         <v>8</v>
       </c>
@@ -710,8 +717,8 @@
       <c r="L7">
         <v>3</v>
       </c>
-      <c r="M7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="M7" s="4"/>
+      <c r="O7" s="4"/>
       <c r="P7">
         <v>8</v>
       </c>
@@ -724,8 +731,8 @@
       <c r="S7">
         <v>3</v>
       </c>
-      <c r="T7" s="2"/>
-      <c r="V7" s="2"/>
+      <c r="T7" s="4"/>
+      <c r="V7" s="4"/>
       <c r="W7">
         <v>8</v>
       </c>
@@ -738,10 +745,10 @@
       <c r="Z7">
         <v>3</v>
       </c>
-      <c r="AA7" s="2"/>
+      <c r="AA7" s="4"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="2"/>
+      <c r="A8" s="4"/>
       <c r="B8">
         <v>9</v>
       </c>
@@ -754,8 +761,8 @@
       <c r="E8">
         <v>4</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="F8" s="4"/>
+      <c r="H8" s="4"/>
       <c r="I8">
         <v>9</v>
       </c>
@@ -768,8 +775,8 @@
       <c r="L8">
         <v>4</v>
       </c>
-      <c r="M8" s="2"/>
-      <c r="O8" s="2"/>
+      <c r="M8" s="4"/>
+      <c r="O8" s="4"/>
       <c r="P8">
         <v>9</v>
       </c>
@@ -782,8 +789,8 @@
       <c r="S8">
         <v>4</v>
       </c>
-      <c r="T8" s="2"/>
-      <c r="V8" s="2"/>
+      <c r="T8" s="4"/>
+      <c r="V8" s="4"/>
       <c r="W8">
         <v>9</v>
       </c>
@@ -796,10 +803,10 @@
       <c r="Z8">
         <v>4</v>
       </c>
-      <c r="AA8" s="2"/>
+      <c r="AA8" s="4"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="2"/>
+      <c r="A9" s="4"/>
       <c r="B9">
         <v>10</v>
       </c>
@@ -812,8 +819,8 @@
       <c r="E9">
         <v>5</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="F9" s="4"/>
+      <c r="H9" s="4"/>
       <c r="I9">
         <v>10</v>
       </c>
@@ -826,8 +833,8 @@
       <c r="L9">
         <v>5</v>
       </c>
-      <c r="M9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="M9" s="4"/>
+      <c r="O9" s="4"/>
       <c r="P9">
         <v>10</v>
       </c>
@@ -840,8 +847,8 @@
       <c r="S9">
         <v>5</v>
       </c>
-      <c r="T9" s="2"/>
-      <c r="V9" s="2"/>
+      <c r="T9" s="4"/>
+      <c r="V9" s="4"/>
       <c r="W9">
         <v>10</v>
       </c>
@@ -854,137 +861,137 @@
       <c r="Z9">
         <v>5</v>
       </c>
-      <c r="AA9" s="2"/>
+      <c r="AA9" s="4"/>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="AA10" s="2"/>
+      <c r="A10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="AA10" s="4"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="AA11" s="2"/>
+      <c r="A11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="AA11" s="4"/>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="AA12" s="2"/>
+      <c r="A12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="AA12" s="4"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="AA13" s="2"/>
+      <c r="A13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="AA13" s="4"/>
     </row>
     <row r="14" spans="1:27">
-      <c r="A14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="AA14" s="2"/>
+      <c r="A14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="AA14" s="4"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="AA15" s="2"/>
+      <c r="A15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="AA15" s="4"/>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="AA16" s="2"/>
+      <c r="A16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="AA16" s="4"/>
     </row>
     <row r="17" spans="1:27">
-      <c r="A17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="AA17" s="2"/>
+      <c r="A17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="AA17" s="4"/>
     </row>
     <row r="18" spans="1:27">
-      <c r="A18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="AA18" s="2"/>
+      <c r="A18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="AA18" s="4"/>
     </row>
     <row r="19" spans="1:27">
-      <c r="A19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="AA19" s="2"/>
+      <c r="A19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="AA19" s="4"/>
     </row>
     <row r="20" spans="1:27">
-      <c r="A20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="AA20" s="2"/>
+      <c r="A20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="AA20" s="4"/>
     </row>
     <row r="21" spans="1:27">
-      <c r="A21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="AA21" s="2"/>
+      <c r="A21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="AA21" s="4"/>
     </row>
     <row r="22" spans="1:27">
-      <c r="A22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="AA22" s="2"/>
+      <c r="A22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="AA22" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1009,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5:O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1049,7 +1056,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
+      <c r="G1" s="2"/>
       <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1058,7 +1065,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
-      <c r="N1" s="4"/>
+      <c r="N1" s="2"/>
       <c r="O1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1067,7 +1074,7 @@
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
-      <c r="U1" s="4"/>
+      <c r="U1" s="2"/>
       <c r="V1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1084,21 +1091,21 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="4"/>
+      <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
-      <c r="U2" s="4"/>
+      <c r="U2" s="2"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
@@ -1113,21 +1120,21 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="4"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
-      <c r="U3" s="4"/>
+      <c r="U3" s="2"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
@@ -1146,7 +1153,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
@@ -1157,7 +1164,7 @@
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="4"/>
+      <c r="N4" s="2"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1" t="s">
@@ -1168,7 +1175,7 @@
       </c>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="4"/>
+      <c r="U4" s="2"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1" t="s">
@@ -1181,999 +1188,1275 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>85.4</v>
+        <v>24</v>
+      </c>
+      <c r="C5" s="5">
+        <v>83.2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>87.3</v>
       </c>
       <c r="E5">
         <v>25</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>87.6</v>
+        <v>24</v>
+      </c>
+      <c r="J5" s="5">
+        <v>70.3</v>
+      </c>
+      <c r="K5" s="5">
+        <v>89.6</v>
       </c>
       <c r="L5">
         <v>25</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="2" t="s">
+      <c r="N5" s="2"/>
+      <c r="O5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>91.1</v>
+        <v>24</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>63</v>
+      </c>
+      <c r="R5" s="5">
+        <v>92.2</v>
       </c>
       <c r="S5">
         <v>25</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="T5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U5" s="4"/>
-      <c r="V5" s="2" t="s">
+      <c r="U5" s="2"/>
+      <c r="V5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="W5">
-        <v>1</v>
-      </c>
-      <c r="Y5">
-        <v>87.2</v>
+        <v>24</v>
+      </c>
+      <c r="X5" s="5">
+        <v>57.9</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>88.7</v>
       </c>
       <c r="Z5">
         <v>25</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="AA5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="2"/>
+      <c r="A6" s="4"/>
       <c r="B6">
-        <f>B5+1</f>
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>82.4</v>
+        <f>B5-1</f>
+        <v>23</v>
+      </c>
+      <c r="C6" s="5">
+        <v>82.5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>83.8</v>
       </c>
       <c r="E6">
         <f>E5+1</f>
         <v>26</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="2"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="4"/>
       <c r="I6">
-        <f>I5+1</f>
-        <v>2</v>
-      </c>
-      <c r="K6">
-        <v>84.8</v>
+        <f>I5-1</f>
+        <v>23</v>
+      </c>
+      <c r="J6" s="5">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="K6" s="5">
+        <v>86.3</v>
       </c>
       <c r="L6">
         <f>L5+1</f>
         <v>26</v>
       </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="2"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="4"/>
       <c r="P6">
-        <f>P5+1</f>
-        <v>2</v>
-      </c>
-      <c r="R6">
-        <v>88.6</v>
+        <f>P5-1</f>
+        <v>23</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>62.6</v>
+      </c>
+      <c r="R6" s="5">
+        <v>89.2</v>
       </c>
       <c r="S6">
         <f>S5+1</f>
         <v>26</v>
       </c>
-      <c r="T6" s="2"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="2"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="4"/>
       <c r="W6">
-        <f>W5+1</f>
-        <v>2</v>
-      </c>
-      <c r="Y6">
-        <v>85.2</v>
+        <f>W5-1</f>
+        <v>23</v>
+      </c>
+      <c r="X6" s="5">
+        <v>58.8</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>86</v>
       </c>
       <c r="Z6">
         <f>Z5+1</f>
         <v>26</v>
       </c>
-      <c r="AA6" s="2"/>
+      <c r="AA6" s="4"/>
     </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="2"/>
+      <c r="A7" s="4"/>
       <c r="B7">
-        <f t="shared" ref="B7:B28" si="0">B6+1</f>
-        <v>3</v>
+        <f t="shared" ref="B7:B28" si="0">B6-1</f>
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>67.599999999999994</v>
       </c>
       <c r="D7">
-        <v>78.900000000000006</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="E7">
         <f t="shared" ref="E7:E28" si="1">E6+1</f>
         <v>27</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="2"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
       <c r="I7">
-        <f t="shared" ref="I7:I28" si="2">I6+1</f>
-        <v>3</v>
+        <f t="shared" ref="I7:I28" si="2">I6-1</f>
+        <v>22</v>
+      </c>
+      <c r="J7">
+        <v>50.9</v>
       </c>
       <c r="K7">
-        <v>81.5</v>
+        <v>82.3</v>
       </c>
       <c r="L7">
         <f t="shared" ref="L7:L28" si="3">L6+1</f>
         <v>27</v>
       </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="2"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="4"/>
       <c r="P7">
-        <f t="shared" ref="P7:P28" si="4">P6+1</f>
-        <v>3</v>
+        <f t="shared" ref="P7:P28" si="4">P6-1</f>
+        <v>22</v>
+      </c>
+      <c r="Q7">
+        <v>58.5</v>
       </c>
       <c r="R7">
-        <v>85.5</v>
+        <v>85.4</v>
       </c>
       <c r="S7">
         <f t="shared" ref="S7:S28" si="5">S6+1</f>
         <v>27</v>
       </c>
-      <c r="T7" s="2"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="2"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="4"/>
       <c r="W7">
-        <f t="shared" ref="W7:W28" si="6">W6+1</f>
-        <v>3</v>
+        <f t="shared" ref="W7:W28" si="6">W6-1</f>
+        <v>22</v>
+      </c>
+      <c r="X7">
+        <v>53</v>
       </c>
       <c r="Y7">
-        <v>82.2</v>
+        <v>82.4</v>
       </c>
       <c r="Z7">
         <f t="shared" ref="Z7:Z28" si="7">Z6+1</f>
         <v>27</v>
       </c>
-      <c r="AA7" s="2"/>
+      <c r="AA7" s="4"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="2"/>
+      <c r="A8" s="4"/>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>63.9</v>
+      </c>
+      <c r="D8">
+        <v>77.900000000000006</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="2"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="4"/>
       <c r="I8">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="J8">
+        <v>38.5</v>
+      </c>
+      <c r="K8">
+        <v>80.599999999999994</v>
       </c>
       <c r="L8">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="2"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="4"/>
       <c r="P8">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="Q8">
+        <v>56.1</v>
+      </c>
+      <c r="R8">
+        <v>84</v>
       </c>
       <c r="S8">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="T8" s="2"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="2"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="4"/>
       <c r="W8">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="X8">
+        <v>50.2</v>
+      </c>
+      <c r="Y8">
+        <v>81</v>
       </c>
       <c r="Z8">
         <f t="shared" si="7"/>
         <v>28</v>
       </c>
-      <c r="AA8" s="2"/>
+      <c r="AA8" s="4"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="2"/>
+      <c r="A9" s="4"/>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>61.4</v>
+      </c>
+      <c r="D9">
+        <v>75.8</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="2"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="4"/>
       <c r="I9">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="J9">
+        <v>39.1</v>
+      </c>
+      <c r="K9">
+        <v>78.599999999999994</v>
       </c>
       <c r="L9">
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="2"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="4"/>
       <c r="P9">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="Q9">
+        <v>55.3</v>
+      </c>
+      <c r="R9">
+        <v>82</v>
       </c>
       <c r="S9">
         <f t="shared" si="5"/>
         <v>29</v>
       </c>
-      <c r="T9" s="2"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="2"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="4"/>
       <c r="W9">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="X9">
+        <v>48.8</v>
+      </c>
+      <c r="Y9">
+        <v>79.099999999999994</v>
       </c>
       <c r="Z9">
         <f t="shared" si="7"/>
         <v>29</v>
       </c>
-      <c r="AA9" s="2"/>
+      <c r="AA9" s="4"/>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="2"/>
+      <c r="A10" s="4"/>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>59</v>
+      </c>
+      <c r="D10">
+        <v>74.3</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="2"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="4"/>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="J10">
+        <v>47.2</v>
+      </c>
+      <c r="K10">
+        <v>77</v>
       </c>
       <c r="L10">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="2"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="4"/>
       <c r="P10">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="Q10">
+        <v>52.4</v>
+      </c>
+      <c r="R10">
+        <v>80.5</v>
       </c>
       <c r="S10">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="T10" s="2"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="2"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="4"/>
       <c r="W10">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="X10">
+        <v>44.6</v>
+      </c>
+      <c r="Y10">
+        <v>77.599999999999994</v>
       </c>
       <c r="Z10">
         <f t="shared" si="7"/>
         <v>30</v>
       </c>
-      <c r="AA10" s="2"/>
+      <c r="AA10" s="4"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="2"/>
+      <c r="A11" s="4"/>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>56.9</v>
+      </c>
+      <c r="D11">
+        <v>73</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="2"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="4"/>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="J11">
+        <v>49.6</v>
+      </c>
+      <c r="K11">
+        <v>75.8</v>
       </c>
       <c r="L11">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="2"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="4"/>
       <c r="P11">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="Q11">
+        <v>53.2</v>
+      </c>
+      <c r="R11">
+        <v>79.2</v>
       </c>
       <c r="S11">
         <f t="shared" si="5"/>
         <v>31</v>
       </c>
-      <c r="T11" s="2"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="2"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="4"/>
       <c r="W11">
         <f t="shared" si="6"/>
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="X11">
+        <v>44.3</v>
+      </c>
+      <c r="Y11">
+        <v>76.5</v>
       </c>
       <c r="Z11">
         <f t="shared" si="7"/>
         <v>31</v>
       </c>
-      <c r="AA11" s="2"/>
+      <c r="AA11" s="4"/>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="2"/>
+      <c r="A12" s="4"/>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>56.4</v>
+      </c>
+      <c r="D12">
+        <v>71.7</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="2"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="4"/>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="J12">
+        <v>50.4</v>
+      </c>
+      <c r="K12">
+        <v>74.400000000000006</v>
       </c>
       <c r="L12">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="2"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="4"/>
       <c r="P12">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="Q12">
+        <v>51.8</v>
+      </c>
+      <c r="R12">
+        <v>78</v>
       </c>
       <c r="S12">
         <f t="shared" si="5"/>
         <v>32</v>
       </c>
-      <c r="T12" s="2"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="2"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="4"/>
       <c r="W12">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="X12">
+        <v>41.8</v>
+      </c>
+      <c r="Y12">
+        <v>75.3</v>
       </c>
       <c r="Z12">
         <f t="shared" si="7"/>
         <v>32</v>
       </c>
-      <c r="AA12" s="2"/>
+      <c r="AA12" s="4"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="2"/>
+      <c r="A13" s="4"/>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>55.9</v>
+      </c>
+      <c r="D13">
+        <v>70.900000000000006</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="2"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="4"/>
       <c r="I13">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="J13">
+        <v>51.6</v>
+      </c>
+      <c r="K13">
+        <v>73.5</v>
       </c>
       <c r="L13">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="2"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="4"/>
       <c r="P13">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="Q13">
+        <v>49.2</v>
+      </c>
+      <c r="R13">
+        <v>77.2</v>
       </c>
       <c r="S13">
         <f t="shared" si="5"/>
         <v>33</v>
       </c>
-      <c r="T13" s="2"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="2"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="4"/>
       <c r="W13">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="X13">
+        <v>38.5</v>
+      </c>
+      <c r="Y13">
+        <v>74.400000000000006</v>
       </c>
       <c r="Z13">
         <f t="shared" si="7"/>
         <v>33</v>
       </c>
-      <c r="AA13" s="2"/>
+      <c r="AA13" s="4"/>
     </row>
     <row r="14" spans="1:27">
-      <c r="A14" s="2"/>
+      <c r="A14" s="4"/>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>55.4</v>
+      </c>
+      <c r="D14">
+        <v>70</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="2"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="4"/>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="J14">
+        <v>51.4</v>
+      </c>
+      <c r="K14">
+        <v>72.599999999999994</v>
       </c>
       <c r="L14">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="2"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="4"/>
       <c r="P14">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="Q14">
+        <v>52.1</v>
+      </c>
+      <c r="R14">
+        <v>76.2</v>
       </c>
       <c r="S14">
         <f t="shared" si="5"/>
         <v>34</v>
       </c>
-      <c r="T14" s="2"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="2"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="4"/>
       <c r="W14">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="X14">
+        <v>39.9</v>
+      </c>
+      <c r="Y14">
+        <v>73.400000000000006</v>
       </c>
       <c r="Z14">
         <f t="shared" si="7"/>
         <v>34</v>
       </c>
-      <c r="AA14" s="2"/>
+      <c r="AA14" s="4"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="2"/>
+      <c r="A15" s="4"/>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>55.2</v>
+      </c>
+      <c r="D15">
+        <v>69</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="2"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="4"/>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <v>51.5</v>
+      </c>
+      <c r="K15">
+        <v>71.7</v>
       </c>
       <c r="L15">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="2"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="4"/>
       <c r="P15">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="Q15">
+        <v>51.9</v>
+      </c>
+      <c r="R15">
+        <v>75</v>
       </c>
       <c r="S15">
         <f t="shared" si="5"/>
         <v>35</v>
       </c>
-      <c r="T15" s="2"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="2"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="4"/>
       <c r="W15">
         <f t="shared" si="6"/>
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="X15">
+        <v>40.4</v>
+      </c>
+      <c r="Y15">
+        <v>72.599999999999994</v>
       </c>
       <c r="Z15">
         <f t="shared" si="7"/>
         <v>35</v>
       </c>
-      <c r="AA15" s="2"/>
+      <c r="AA15" s="4"/>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="2"/>
+      <c r="A16" s="4"/>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>54.8</v>
+      </c>
+      <c r="D16">
+        <v>68.400000000000006</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="2"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="4"/>
       <c r="I16">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J16">
+        <v>51.2</v>
+      </c>
+      <c r="K16">
+        <v>71.099999999999994</v>
       </c>
       <c r="L16">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="2"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="4"/>
       <c r="P16">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="Q16">
+        <v>51.2</v>
+      </c>
+      <c r="R16">
+        <v>74.3</v>
       </c>
       <c r="S16">
         <f t="shared" si="5"/>
         <v>36</v>
       </c>
-      <c r="T16" s="2"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="2"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="4"/>
       <c r="W16">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="X16">
+        <v>39</v>
+      </c>
+      <c r="Y16">
+        <v>72</v>
       </c>
       <c r="Z16">
         <f t="shared" si="7"/>
         <v>36</v>
       </c>
-      <c r="AA16" s="2"/>
+      <c r="AA16" s="4"/>
     </row>
     <row r="17" spans="1:27">
-      <c r="A17" s="2"/>
+      <c r="A17" s="4"/>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>54</v>
+      </c>
+      <c r="D17">
+        <v>67.400000000000006</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="2"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="4"/>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="J17">
+        <v>50.4</v>
+      </c>
+      <c r="K17">
+        <v>70.3</v>
       </c>
       <c r="L17">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="2"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="4"/>
       <c r="P17">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="Q17">
+        <v>51.3</v>
+      </c>
+      <c r="R17">
+        <v>73.8</v>
       </c>
       <c r="S17">
         <f t="shared" si="5"/>
         <v>37</v>
       </c>
-      <c r="T17" s="2"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="2"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="4"/>
       <c r="W17">
         <f t="shared" si="6"/>
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="X17">
+        <v>42.1</v>
+      </c>
+      <c r="Y17">
+        <v>71.3</v>
       </c>
       <c r="Z17">
         <f t="shared" si="7"/>
         <v>37</v>
       </c>
-      <c r="AA17" s="2"/>
+      <c r="AA17" s="4"/>
     </row>
     <row r="18" spans="1:27">
-      <c r="A18" s="2"/>
+      <c r="A18" s="4"/>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="2"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="4"/>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L18">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="2"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="4"/>
       <c r="P18">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="S18">
         <f t="shared" si="5"/>
         <v>38</v>
       </c>
-      <c r="T18" s="2"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="2"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="4"/>
       <c r="W18">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="Z18">
         <f t="shared" si="7"/>
         <v>38</v>
       </c>
-      <c r="AA18" s="2"/>
+      <c r="AA18" s="4"/>
     </row>
     <row r="19" spans="1:27">
-      <c r="A19" s="2"/>
+      <c r="A19" s="4"/>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="2"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="4"/>
       <c r="I19">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L19">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="M19" s="2"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="2"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="4"/>
       <c r="P19">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="S19">
         <f t="shared" si="5"/>
         <v>39</v>
       </c>
-      <c r="T19" s="2"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="2"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="4"/>
       <c r="W19">
         <f t="shared" si="6"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="Z19">
         <f t="shared" si="7"/>
         <v>39</v>
       </c>
-      <c r="AA19" s="2"/>
+      <c r="AA19" s="4"/>
     </row>
     <row r="20" spans="1:27">
-      <c r="A20" s="2"/>
+      <c r="A20" s="4"/>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="2"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="4"/>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="L20">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="2"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="4"/>
       <c r="P20">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="S20">
         <f t="shared" si="5"/>
         <v>40</v>
       </c>
-      <c r="T20" s="2"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="2"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="4"/>
       <c r="W20">
         <f t="shared" si="6"/>
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="Z20">
         <f t="shared" si="7"/>
         <v>40</v>
       </c>
-      <c r="AA20" s="2"/>
+      <c r="AA20" s="4"/>
     </row>
     <row r="21" spans="1:27">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="2"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="4"/>
       <c r="I21">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="L21">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="2"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="4"/>
       <c r="P21">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="S21">
         <f t="shared" si="5"/>
         <v>41</v>
       </c>
-      <c r="T21" s="2"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="2"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="4"/>
       <c r="W21">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="Z21">
         <f t="shared" si="7"/>
         <v>41</v>
       </c>
-      <c r="AA21" s="2"/>
+      <c r="AA21" s="4"/>
     </row>
     <row r="22" spans="1:27">
-      <c r="A22" s="2"/>
+      <c r="A22" s="4"/>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="2"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="4"/>
       <c r="I22">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="L22">
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="2"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="4"/>
       <c r="P22">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="S22">
         <f t="shared" si="5"/>
         <v>42</v>
       </c>
-      <c r="T22" s="2"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="2"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="4"/>
       <c r="W22">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="Z22">
         <f t="shared" si="7"/>
         <v>42</v>
       </c>
-      <c r="AA22" s="2"/>
+      <c r="AA22" s="4"/>
     </row>
     <row r="23" spans="1:27">
-      <c r="A23" s="2"/>
+      <c r="A23" s="4"/>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="2"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="4"/>
       <c r="I23">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L23">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="2"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="4"/>
       <c r="P23">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="S23">
         <f t="shared" si="5"/>
         <v>43</v>
       </c>
-      <c r="T23" s="2"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="2"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="4"/>
       <c r="W23">
         <f t="shared" si="6"/>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Z23">
         <f t="shared" si="7"/>
         <v>43</v>
       </c>
-      <c r="AA23" s="2"/>
+      <c r="AA23" s="4"/>
     </row>
     <row r="24" spans="1:27">
-      <c r="A24" s="2"/>
+      <c r="A24" s="4"/>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="2"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="4"/>
       <c r="I24">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="L24">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="M24" s="2"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="2"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="4"/>
       <c r="P24">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="S24">
         <f t="shared" si="5"/>
         <v>44</v>
       </c>
-      <c r="T24" s="2"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="2"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="4"/>
       <c r="W24">
         <f t="shared" si="6"/>
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="Z24">
         <f t="shared" si="7"/>
         <v>44</v>
       </c>
-      <c r="AA24" s="2"/>
+      <c r="AA24" s="4"/>
     </row>
     <row r="25" spans="1:27">
-      <c r="A25" s="2"/>
+      <c r="A25" s="4"/>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="2"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="4"/>
       <c r="I25">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="L25">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="M25" s="2"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="2"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="4"/>
       <c r="P25">
         <f t="shared" si="4"/>
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="S25">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
-      <c r="T25" s="2"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="2"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="4"/>
       <c r="W25">
         <f t="shared" si="6"/>
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="Z25">
         <f t="shared" si="7"/>
         <v>45</v>
       </c>
-      <c r="AA25" s="2"/>
+      <c r="AA25" s="4"/>
     </row>
     <row r="26" spans="1:27">
-      <c r="A26" s="2"/>
+      <c r="A26" s="4"/>
       <c r="B26">
-        <f>B25+1</f>
-        <v>22</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>76.7</v>
@@ -2182,12 +2465,12 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="2"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="4"/>
       <c r="I26">
-        <f>I25+1</f>
-        <v>22</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="J26">
         <v>63.5</v>
@@ -2196,12 +2479,12 @@
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
-      <c r="M26" s="2"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="2"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="4"/>
       <c r="P26">
-        <f>P25+1</f>
-        <v>22</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="Q26">
         <v>62.1</v>
@@ -2210,12 +2493,12 @@
         <f t="shared" si="5"/>
         <v>46</v>
       </c>
-      <c r="T26" s="2"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="2"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="4"/>
       <c r="W26">
-        <f>W25+1</f>
-        <v>22</v>
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="X26">
         <v>56.2</v>
@@ -2224,13 +2507,13 @@
         <f t="shared" si="7"/>
         <v>46</v>
       </c>
-      <c r="AA26" s="2"/>
+      <c r="AA26" s="4"/>
     </row>
     <row r="27" spans="1:27">
-      <c r="A27" s="2"/>
+      <c r="A27" s="4"/>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C27">
         <v>79.900000000000006</v>
@@ -2239,12 +2522,12 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="2"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="4"/>
       <c r="I27">
-        <f t="shared" ref="I27:I28" si="8">I26+1</f>
-        <v>23</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="J27">
         <v>66.7</v>
@@ -2253,12 +2536,12 @@
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="2"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="4"/>
       <c r="P27">
-        <f t="shared" ref="P27:P28" si="9">P26+1</f>
-        <v>23</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="Q27">
         <v>62.7</v>
@@ -2267,12 +2550,12 @@
         <f t="shared" si="5"/>
         <v>47</v>
       </c>
-      <c r="T27" s="2"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="2"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="4"/>
       <c r="W27">
-        <f t="shared" ref="W27:W28" si="10">W26+1</f>
-        <v>23</v>
+        <f t="shared" si="6"/>
+        <v>2</v>
       </c>
       <c r="X27">
         <v>57.5</v>
@@ -2281,13 +2564,13 @@
         <f t="shared" si="7"/>
         <v>47</v>
       </c>
-      <c r="AA27" s="2"/>
+      <c r="AA27" s="4"/>
     </row>
     <row r="28" spans="1:27">
-      <c r="A28" s="2"/>
+      <c r="A28" s="4"/>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>82</v>
@@ -2296,12 +2579,12 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="2"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="4"/>
       <c r="I28">
-        <f t="shared" si="8"/>
-        <v>24</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="J28">
         <v>69</v>
@@ -2310,12 +2593,12 @@
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="M28" s="2"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="2"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="4"/>
       <c r="P28">
-        <f t="shared" si="9"/>
-        <v>24</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="Q28">
         <v>64</v>
@@ -2324,12 +2607,12 @@
         <f t="shared" si="5"/>
         <v>48</v>
       </c>
-      <c r="T28" s="2"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="2"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="4"/>
       <c r="W28">
-        <f t="shared" si="10"/>
-        <v>24</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="X28">
         <v>58</v>
@@ -2338,15 +2621,10 @@
         <f t="shared" si="7"/>
         <v>48</v>
       </c>
-      <c r="AA28" s="2"/>
+      <c r="AA28" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A5:A28"/>
-    <mergeCell ref="F5:F28"/>
-    <mergeCell ref="H5:H28"/>
-    <mergeCell ref="M5:M28"/>
-    <mergeCell ref="O5:O28"/>
     <mergeCell ref="T5:T28"/>
     <mergeCell ref="V5:V28"/>
     <mergeCell ref="AA5:AA28"/>
@@ -2354,6 +2632,11 @@
     <mergeCell ref="H1:M3"/>
     <mergeCell ref="O1:T3"/>
     <mergeCell ref="V1:AA3"/>
+    <mergeCell ref="A5:A28"/>
+    <mergeCell ref="F5:F28"/>
+    <mergeCell ref="H5:H28"/>
+    <mergeCell ref="M5:M28"/>
+    <mergeCell ref="O5:O28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>